<commit_message>
Styles, parameters & documentation
# In this commit:

* ForEach documentation and two additional fields dor iterator (`__startOutput` and `__endOutput`)
* Parameters for ForEachCell (and ContinueCell)
* Applying styles

### TODO:

3. working with sheets
6. refactoring - make code simplify, extract methods, clean up code,
7. `SumCell` with pattern `#! SUM [TARGET]` - sum coll in rows from `vm[TARGET].__startOutput` to `vm[TARGET].__endOutput`
8. npm package
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siemi\aProjects\xlsx-template-engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9DB71161-C1B0-408C-91FA-CAC63C48EBEF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3D4BA44C-163B-4B36-91C0-032FD55A3AA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10700" xr2:uid="{2C0B4293-7837-4594-B054-67970614D784}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>to</t>
   </si>
@@ -69,31 +69,28 @@
     <t>#! FINISH</t>
   </si>
   <si>
-    <t>NIESTETY!</t>
-  </si>
-  <si>
     <t>## super.test</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>w1</t>
-  </si>
-  <si>
-    <t>w2</t>
-  </si>
-  <si>
-    <t>przed</t>
-  </si>
-  <si>
-    <t>po</t>
-  </si>
-  <si>
     <t>## i.__index</t>
   </si>
   <si>
     <t>#! CONTINUE i</t>
+  </si>
+  <si>
+    <t>foy</t>
+  </si>
+  <si>
+    <t>## i.__start</t>
+  </si>
+  <si>
+    <t>## i.__end</t>
+  </si>
+  <si>
+    <t>## i.__startOutput</t>
+  </si>
+  <si>
+    <t>## i.__endOutput</t>
   </si>
 </sst>
 </file>
@@ -134,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +162,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -298,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,11 +332,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -333,9 +356,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,13 +673,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BC7ACE-46B4-47B2-BA3A-12797827C4B5}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="9" max="9" width="21.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="21.90625" style="27" customWidth="1"/>
     <col min="10" max="10" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -672,12 +693,7 @@
       <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F2" s="7"/>
@@ -702,7 +718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -725,10 +741,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="24"/>
+      <c r="D6" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="30"/>
       <c r="F6" s="8"/>
       <c r="G6" s="6"/>
       <c r="J6" t="s">
@@ -736,23 +752,21 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="13"/>
       <c r="G7" s="17"/>
       <c r="J7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="7"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="18"/>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" t="s">
-        <v>16</v>
+    <row r="8" spans="1:12" s="23" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="23" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -762,16 +776,14 @@
       <c r="J9" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -782,27 +794,22 @@
         <v>6</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="12"/>
@@ -810,23 +817,20 @@
         <v>8</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>21</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="I11" s="28"/>
       <c r="J11" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E12" s="7"/>
       <c r="J12" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E13" s="7"/>
@@ -835,19 +839,27 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
+      <c r="F14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>19</v>
+      </c>
       <c r="J14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="J15" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Sum & Average loop column, fixes with merged cells
* NEW: SumCell
* NEW: AverageCell
* FIXED: inserting rows causes remove-ing merged cells below
* FIXED: inserted rows hasn't merged cells
* Merging cells when it's necessary

3. working with sheets
6. refactoring - make code simplify, extract methods, clean up code,
8. npm package
9. matching should based on cell instead of value
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siemi\aProjects\xlsx-template-engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3D4BA44C-163B-4B36-91C0-032FD55A3AA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{99C4D2B4-0E88-41CD-AC08-7391C7B02BE5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10700" xr2:uid="{2C0B4293-7837-4594-B054-67970614D784}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>to</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>## i.__endOutput</t>
+  </si>
+  <si>
+    <t>#! SUM i</t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -309,11 +312,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -357,6 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,7 +693,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -864,17 +883,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="7:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G17" s="33" t="s">
+        <v>22</v>
+      </c>
       <c r="J17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="7:10" x14ac:dyDescent="0.35">
       <c r="J18" t="s">
         <v>13</v>
       </c>

</xml_diff>